<commit_message>
Changes such that we can test on dates
</commit_message>
<xml_diff>
--- a/src/main/resources/com/company/rules/inputObjectExample.xlsx
+++ b/src/main/resources/com/company/rules/inputObjectExample.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\workspace\drools-minimum-example\src\test\resources\com\company\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Drools\src\main\resources\com\company\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855A7F0C-91E8-4267-A006-35FD025DE07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7644" yWindow="5280" windowWidth="31536" windowHeight="16812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+  <si>
+    <t>RuleSet</t>
+  </si>
   <si>
     <t>Import</t>
   </si>
   <si>
-    <t>RuleSet</t>
+    <t>RuleTable L&amp;F validation</t>
   </si>
   <si>
     <t>NAME</t>
@@ -42,48 +44,38 @@
     <t>ACTION</t>
   </si>
   <si>
-    <t>RuleTable L&amp;F validation</t>
+    <t>animal : InputObject</t>
+  </si>
+  <si>
+    <t>DyrAlder</t>
   </si>
   <si>
     <t>errorCode</t>
   </si>
   <si>
-    <t>Check_DyrAlder</t>
-  </si>
-  <si>
-    <t>DyrAlder</t>
-  </si>
-  <si>
-    <t>HDY-08277, Dyrets alder er mindre end 8 måned(er)</t>
-  </si>
-  <si>
-    <t>animal.addValidationResult(new ValidationResult("$1","$2"));</t>
-  </si>
-  <si>
-    <t>ruleSet</t>
-  </si>
-  <si>
-    <t>set3</t>
-  </si>
-  <si>
-    <t>input["DyrAlder"] &lt; $param</t>
-  </si>
-  <si>
-    <t>animal:InputObject</t>
+    <t>Check_Date</t>
+  </si>
+  <si>
+    <t>ErrorCode123, ErrorText321, Check_Date</t>
+  </si>
+  <si>
+    <t>System.out.println("$param");</t>
   </si>
   <si>
     <t>com.company.rules.droolsObjectValidation</t>
   </si>
   <si>
-    <t>com.company.model.InputObject,
-com.company.model.ValidationResult</t>
+    <t>com.company.model.InputObject</t>
+  </si>
+  <si>
+    <t>date &lt; $param</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,21 +92,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,18 +118,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -160,7 +139,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -193,22 +184,16 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -217,9 +202,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -229,82 +212,71 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -312,12 +284,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFFF6600"/>
-      <color rgb="FFFFFFCC"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -591,151 +557,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" customWidth="1"/>
-    <col min="4" max="4" width="40.21875" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.33203125" customWidth="1"/>
-    <col min="11" max="11" width="34" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="50.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:15" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="B2" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="18" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="21"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-    </row>
-    <row r="7" spans="1:15" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="B8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="20">
+        <v>44562</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="9">
-        <v>5</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="20"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:C6"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>